<commit_message>
added excel functions and diagram for report
</commit_message>
<xml_diff>
--- a/baseline_decision_score.xlsx
+++ b/baseline_decision_score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philippe T-B\Documents\PythonProject\GTI770_Labo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD930A9-1491-468E-84EF-EB02D51E0C03}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E014FB-8569-4353-9DB9-F7C250A57F65}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,18 +40,12 @@
     <t>Params</t>
   </si>
   <si>
-    <t>C = 10, gamma = 10, kernel = rbf</t>
-  </si>
-  <si>
     <t>Bayes (Gaussian)</t>
   </si>
   <si>
     <t>priors=None</t>
   </si>
   <si>
-    <t>criterion='entropy', max_depth=15, min_samples_leaf=1</t>
-  </si>
-  <si>
     <t>Dataset</t>
   </si>
   <si>
@@ -65,6 +59,12 @@
   </si>
   <si>
     <t>JMIR Derivatives</t>
+  </si>
+  <si>
+    <t>C = 1, gamma = 10, kernel = rbf</t>
+  </si>
+  <si>
+    <t>criterion='entropy', max_depth=14, min_samples_leaf=1</t>
   </si>
 </sst>
 </file>
@@ -389,13 +389,13 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="15.7265625" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
     <col min="4" max="4" width="49.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -404,10 +404,10 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -421,16 +421,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -444,13 +444,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -464,13 +464,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>0</v>

</xml_diff>